<commit_message>
sample summary output for filescan
</commit_message>
<xml_diff>
--- a/testreport/attributes.xlsx
+++ b/testreport/attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win 10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/huy_nq210427_sis_hust_edu_vn/Documents/Documents/GitHub/oop-bee/testreport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70740F6A-895B-4027-90C6-9AF114B6D568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{70740F6A-895B-4027-90C6-9AF114B6D568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75AC310C-2D1A-46C2-8C18-A73A915D53E0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BD7BB095-AAAE-409B-AF0F-A91403626AF3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD7BB095-AAAE-409B-AF0F-A91403626AF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
   <si>
     <t>type_description</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>alias</t>
   </si>
 </sst>
 </file>
@@ -384,14 +387,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8336376-DD56-42FE-B04D-3D6C770199B7}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,18 +728,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="4"/>
+      <c r="H1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1237,10 +1244,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1250,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B050D7B-DAAC-4622-8BFC-B53EE987AC66}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1264,22 +1272,22 @@
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1288,19 +1296,19 @@
         <f t="array" ref="A2:A60">_xlfn.UNIQUE(_xlfn.VSTACK(Sheet1!A2:A43,Sheet1!D2:D43,Sheet1!G2:G43,Sheet1!J2:J43))</f>
         <v>type_description</v>
       </c>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>IF(IFERROR(MATCH(A2,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>IF(IFERROR(MATCH($A2,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>IF(IFERROR(MATCH($A2,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>IF(IFERROR(MATCH($A2,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -1309,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <v>tlsh</v>
       </c>
@@ -1334,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <v>vhash</v>
       </c>
@@ -1363,19 +1371,19 @@
       <c r="A5" s="1" t="str">
         <v>type_tags</v>
       </c>
-      <c r="B5" s="5" t="str">
+      <c r="B5" s="4" t="str">
         <f>IF(IFERROR(MATCH(A5,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="C5" s="4" t="str">
         <f>IF(IFERROR(MATCH($A5,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D5" s="5" t="str">
+      <c r="D5" s="4" t="str">
         <f>IF(IFERROR(MATCH($A5,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E5" s="5" t="str">
+      <c r="E5" s="4" t="str">
         <f>IF(IFERROR(MATCH($A5,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -1383,11 +1391,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <v>crowdsourced_yara_results</v>
       </c>
@@ -1413,47 +1421,50 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="str">
+      <c r="A7" s="7" t="str">
         <v>names</v>
       </c>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="4" t="str">
         <f>IF(IFERROR(MATCH(A7,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C7" s="5" t="str">
+      <c r="C7" s="4" t="str">
         <f>IF(IFERROR(MATCH($A7,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="D7" s="4" t="str">
         <f>IF(IFERROR(MATCH($A7,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E7" s="5" t="str">
+      <c r="E7" s="4" t="str">
         <f>IF(IFERROR(MATCH($A7,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <v>last_modification_date</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="4" t="str">
         <f>IF(IFERROR(MATCH(A8,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C8" s="5" t="str">
+      <c r="C8" s="4" t="str">
         <f>IF(IFERROR(MATCH($A8,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D8" s="5" t="str">
+      <c r="D8" s="4" t="str">
         <f>IF(IFERROR(MATCH($A8,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E8" s="5" t="str">
+      <c r="E8" s="4" t="str">
         <f>IF(IFERROR(MATCH($A8,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1462,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <v>times_submitted</v>
       </c>
@@ -1488,22 +1499,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="7" t="str">
         <v>total_votes</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="4" t="str">
         <f>IF(IFERROR(MATCH(A10,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C10" s="5" t="str">
+      <c r="C10" s="4" t="str">
         <f>IF(IFERROR(MATCH($A10,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D10" s="5" t="str">
+      <c r="D10" s="4" t="str">
         <f>IF(IFERROR(MATCH($A10,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E10" s="5" t="str">
+      <c r="E10" s="4" t="str">
         <f>IF(IFERROR(MATCH($A10,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1516,19 +1527,19 @@
       <c r="A11" s="1" t="str">
         <v>size</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="4" t="str">
         <f>IF(IFERROR(MATCH(A11,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C11" s="5" t="str">
+      <c r="C11" s="4" t="str">
         <f>IF(IFERROR(MATCH($A11,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D11" s="5" t="str">
+      <c r="D11" s="4" t="str">
         <f>IF(IFERROR(MATCH($A11,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" s="4" t="str">
         <f>IF(IFERROR(MATCH($A11,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -1537,8 +1548,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="str">
+    <row r="12" spans="1:7" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="str">
         <v>type_extension</v>
       </c>
       <c r="B12" s="5" t="str">
@@ -1557,12 +1568,12 @@
         <f>IF(IFERROR(MATCH($A12,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <v>last_submission_date</v>
       </c>
@@ -1587,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <v>unique_sources</v>
       </c>
@@ -1638,22 +1649,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="7" t="str">
         <v>last_analysis_results</v>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B16" s="4" t="str">
         <f>IF(IFERROR(MATCH(A16,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C16" s="5" t="str">
+      <c r="C16" s="4" t="str">
         <f>IF(IFERROR(MATCH($A16,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D16" s="5" t="str">
+      <c r="D16" s="4" t="str">
         <f>IF(IFERROR(MATCH($A16,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E16" s="5" t="str">
+      <c r="E16" s="4" t="str">
         <f>IF(IFERROR(MATCH($A16,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1663,22 +1674,22 @@
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="str">
+      <c r="A17" s="7" t="str">
         <v>last_analysis_stats</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="4" t="str">
         <f>IF(IFERROR(MATCH(A17,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="4" t="str">
         <f>IF(IFERROR(MATCH($A17,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D17" s="5" t="str">
+      <c r="D17" s="4" t="str">
         <f>IF(IFERROR(MATCH($A17,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E17" s="5" t="str">
+      <c r="E17" s="4" t="str">
         <f>IF(IFERROR(MATCH($A17,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1687,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <v>trid</v>
       </c>
@@ -1712,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <v>sha256</v>
       </c>
@@ -1738,22 +1749,22 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="7" t="str">
         <v>tags</v>
       </c>
-      <c r="B20" s="5" t="str">
+      <c r="B20" s="4" t="str">
         <f>IF(IFERROR(MATCH(A20,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C20" s="5" t="str">
+      <c r="C20" s="4" t="str">
         <f>IF(IFERROR(MATCH($A20,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D20" s="5" t="str">
+      <c r="D20" s="4" t="str">
         <f>IF(IFERROR(MATCH($A20,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E20" s="5" t="str">
+      <c r="E20" s="4" t="str">
         <f>IF(IFERROR(MATCH($A20,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1766,19 +1777,19 @@
       <c r="A21" s="1" t="str">
         <v>last_analysis_date</v>
       </c>
-      <c r="B21" s="5" t="str">
+      <c r="B21" s="4" t="str">
         <f>IF(IFERROR(MATCH(A21,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C21" s="5" t="str">
+      <c r="C21" s="4" t="str">
         <f>IF(IFERROR(MATCH($A21,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D21" s="5" t="str">
+      <c r="D21" s="4" t="str">
         <f>IF(IFERROR(MATCH($A21,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E21" s="5" t="str">
+      <c r="E21" s="4" t="str">
         <f>IF(IFERROR(MATCH($A21,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1787,7 +1798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <v>first_submission_date</v>
       </c>
@@ -1812,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <v>ssdeep</v>
       </c>
@@ -1837,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <v>md5</v>
       </c>
@@ -1862,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <v>sha1</v>
       </c>
@@ -1887,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <v>magic</v>
       </c>
@@ -1916,19 +1927,19 @@
       <c r="A27" s="1" t="str">
         <v>meaningful_name</v>
       </c>
-      <c r="B27" s="5" t="str">
+      <c r="B27" s="4" t="str">
         <f>IF(IFERROR(MATCH(A27,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C27" s="5" t="str">
+      <c r="C27" s="4" t="str">
         <f>IF(IFERROR(MATCH($A27,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D27" s="5" t="str">
+      <c r="D27" s="4" t="str">
         <f>IF(IFERROR(MATCH($A27,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E27" s="5" t="str">
+      <c r="E27" s="4" t="str">
         <f>IF(IFERROR(MATCH($A27,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -1936,7 +1947,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="6" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1944,19 +1955,19 @@
       <c r="A28" s="1" t="str">
         <v>reputation</v>
       </c>
-      <c r="B28" s="5" t="str">
+      <c r="B28" s="4" t="str">
         <f>IF(IFERROR(MATCH(A28,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C28" s="5" t="str">
+      <c r="C28" s="4" t="str">
         <f>IF(IFERROR(MATCH($A28,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D28" s="5" t="str">
+      <c r="D28" s="4" t="str">
         <f>IF(IFERROR(MATCH($A28,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E28" s="5" t="str">
+      <c r="E28" s="4" t="str">
         <f>IF(IFERROR(MATCH($A28,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1969,19 +1980,19 @@
       <c r="A29" s="1" t="str">
         <v>type</v>
       </c>
-      <c r="B29" s="5" t="str">
+      <c r="B29" s="4" t="str">
         <f>IF(IFERROR(MATCH(A29,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C29" s="5" t="str">
+      <c r="C29" s="4" t="str">
         <f>IF(IFERROR(MATCH($A29,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D29" s="5" t="str">
+      <c r="D29" s="4" t="str">
         <f>IF(IFERROR(MATCH($A29,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E29" s="5" t="str">
+      <c r="E29" s="4" t="str">
         <f>IF(IFERROR(MATCH($A29,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -1994,19 +2005,19 @@
       <c r="A30" s="1" t="str">
         <v>id</v>
       </c>
-      <c r="B30" s="5" t="str">
+      <c r="B30" s="4" t="str">
         <f>IF(IFERROR(MATCH(A30,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="C30" s="5" t="str">
+      <c r="C30" s="4" t="str">
         <f>IF(IFERROR(MATCH($A30,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D30" s="5" t="str">
+      <c r="D30" s="4" t="str">
         <f>IF(IFERROR(MATCH($A30,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E30" s="5" t="str">
+      <c r="E30" s="4" t="str">
         <f>IF(IFERROR(MATCH($A30,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -2015,7 +2026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <v>links</v>
       </c>
@@ -2040,7 +2051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <v>threat_names</v>
       </c>
@@ -2065,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <v>redirection_chain</v>
       </c>
@@ -2094,19 +2105,19 @@
       <c r="A34" s="1" t="str">
         <v>last_final_url</v>
       </c>
-      <c r="B34" s="5" t="str">
+      <c r="B34" s="4" t="str">
         <f>IF(IFERROR(MATCH(A34,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C34" s="5" t="str">
+      <c r="C34" s="4" t="str">
         <f>IF(IFERROR(MATCH($A34,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D34" s="5" t="str">
+      <c r="D34" s="4" t="str">
         <f>IF(IFERROR(MATCH($A34,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E34" s="5" t="str">
+      <c r="E34" s="4" t="str">
         <f>IF(IFERROR(MATCH($A34,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -2115,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <v>categories</v>
       </c>
@@ -2140,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <v>trackers</v>
       </c>
@@ -2165,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <v>tld</v>
       </c>
@@ -2190,7 +2201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <v>last_http_response_headers</v>
       </c>
@@ -2219,19 +2230,19 @@
       <c r="A39" s="1" t="str">
         <v>last_http_response_content_length</v>
       </c>
-      <c r="B39" s="5" t="str">
+      <c r="B39" s="4" t="str">
         <f>IF(IFERROR(MATCH(A39,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C39" s="5" t="str">
+      <c r="C39" s="4" t="str">
         <f>IF(IFERROR(MATCH($A39,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D39" s="5" t="str">
+      <c r="D39" s="4" t="str">
         <f>IF(IFERROR(MATCH($A39,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E39" s="5" t="str">
+      <c r="E39" s="4" t="str">
         <f>IF(IFERROR(MATCH($A39,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -2240,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <v>last_http_response_content_sha256</v>
       </c>
@@ -2265,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <v>last_http_response_code</v>
       </c>
@@ -2290,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <v>html_meta</v>
       </c>
@@ -2319,19 +2330,19 @@
       <c r="A43" s="1" t="str">
         <v>title</v>
       </c>
-      <c r="B43" s="5" t="str">
+      <c r="B43" s="4" t="str">
         <f>IF(IFERROR(MATCH(A43,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C43" s="5" t="str">
+      <c r="C43" s="4" t="str">
         <f>IF(IFERROR(MATCH($A43,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D43" s="5" t="str">
+      <c r="D43" s="4" t="str">
         <f>IF(IFERROR(MATCH($A43,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E43" s="5" t="str">
+      <c r="E43" s="4" t="str">
         <f>IF(IFERROR(MATCH($A43,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -2344,19 +2355,19 @@
       <c r="A44" s="1" t="str">
         <v>url</v>
       </c>
-      <c r="B44" s="5" t="str">
+      <c r="B44" s="4" t="str">
         <f>IF(IFERROR(MATCH(A44,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C44" s="5" t="str">
+      <c r="C44" s="4" t="str">
         <f>IF(IFERROR(MATCH($A44,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="D44" s="5" t="str">
+      <c r="D44" s="4" t="str">
         <f>IF(IFERROR(MATCH($A44,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E44" s="5" t="str">
+      <c r="E44" s="4" t="str">
         <f>IF(IFERROR(MATCH($A44,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -2364,11 +2375,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <v>regional_internet_registry</v>
       </c>
@@ -2397,19 +2408,19 @@
       <c r="A46" s="1" t="str">
         <v>network</v>
       </c>
-      <c r="B46" s="5" t="str">
+      <c r="B46" s="4" t="str">
         <f>IF(IFERROR(MATCH(A46,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C46" s="5" t="str">
+      <c r="C46" s="4" t="str">
         <f>IF(IFERROR(MATCH($A46,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D46" s="5" t="str">
+      <c r="D46" s="4" t="str">
         <f>IF(IFERROR(MATCH($A46,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E46" s="5" t="str">
+      <c r="E46" s="4" t="str">
         <f>IF(IFERROR(MATCH($A46,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -2417,7 +2428,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G46" s="6" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2425,19 +2436,19 @@
       <c r="A47" s="1" t="str">
         <v>country</v>
       </c>
-      <c r="B47" s="5" t="str">
+      <c r="B47" s="4" t="str">
         <f>IF(IFERROR(MATCH(A47,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C47" s="5" t="str">
+      <c r="C47" s="4" t="str">
         <f>IF(IFERROR(MATCH($A47,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D47" s="5" t="str">
+      <c r="D47" s="4" t="str">
         <f>IF(IFERROR(MATCH($A47,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="E47" s="5" t="str">
+      <c r="E47" s="4" t="str">
         <f>IF(IFERROR(MATCH($A47,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -2446,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <v>as_owner</v>
       </c>
@@ -2471,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <v>asn</v>
       </c>
@@ -2496,7 +2507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <v>continent</v>
       </c>
@@ -2525,19 +2536,19 @@
       <c r="A51" s="1" t="str">
         <v>whois</v>
       </c>
-      <c r="B51" s="5" t="str">
+      <c r="B51" s="4" t="str">
         <f>IF(IFERROR(MATCH(A51,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C51" s="5" t="str">
+      <c r="C51" s="4" t="str">
         <f>IF(IFERROR(MATCH($A51,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D51" s="5" t="str">
+      <c r="D51" s="4" t="str">
         <f>IF(IFERROR(MATCH($A51,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E51" s="5" t="str">
+      <c r="E51" s="4" t="str">
         <f>IF(IFERROR(MATCH($A51,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -2550,19 +2561,19 @@
       <c r="A52" s="1" t="str">
         <v>whois_date</v>
       </c>
-      <c r="B52" s="5" t="str">
+      <c r="B52" s="4" t="str">
         <f>IF(IFERROR(MATCH(A52,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C52" s="5" t="str">
+      <c r="C52" s="4" t="str">
         <f>IF(IFERROR(MATCH($A52,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D52" s="5" t="str">
+      <c r="D52" s="4" t="str">
         <f>IF(IFERROR(MATCH($A52,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E52" s="5" t="str">
+      <c r="E52" s="4" t="str">
         <f>IF(IFERROR(MATCH($A52,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
@@ -2575,19 +2586,19 @@
       <c r="A53" s="1" t="str">
         <v>registrar</v>
       </c>
-      <c r="B53" s="5" t="str">
+      <c r="B53" s="4" t="str">
         <f>IF(IFERROR(MATCH(A53,Sheet1!A:A,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="C53" s="5" t="str">
+      <c r="C53" s="4" t="str">
         <f>IF(IFERROR(MATCH($A53,Sheet1!D:D,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="D53" s="5" t="str">
+      <c r="D53" s="4" t="str">
         <f>IF(IFERROR(MATCH($A53,Sheet1!J:J,0),-1)&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E53" s="5" t="str">
+      <c r="E53" s="4" t="str">
         <f>IF(IFERROR(MATCH($A53,Sheet1!G:G,0),-1)&gt;0,"X","")</f>
         <v/>
       </c>
@@ -2596,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <v>last_dns_records</v>
       </c>
@@ -2621,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <v>last_dns_records_date</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <v>last_https_certificate</v>
       </c>
@@ -2671,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <v>last_https_certificate_date</v>
       </c>
@@ -2696,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <v>jarm</v>
       </c>
@@ -2721,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <v>creation_date</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <v>popularity_ranks</v>
       </c>

</xml_diff>